<commit_message>
POPRAWIONY MANGER, przenosi z w_trakcie
</commit_message>
<xml_diff>
--- a/testy_MANAGER_GIECIA/ListaElementow.xlsx
+++ b/testy_MANAGER_GIECIA/ListaElementow.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,6 +503,38 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>prd.40062106.dld</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Gotowe</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>prd.40662901siatka.dld</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Gotowe</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
POPRAWIONY MANGER, limit, dobrze dzialajaca wersja
</commit_message>
<xml_diff>
--- a/testy_MANAGER_GIECIA/ListaElementow.xlsx
+++ b/testy_MANAGER_GIECIA/ListaElementow.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,7 +467,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Archiwum</t>
+          <t>W trakcie</t>
         </is>
       </c>
     </row>
@@ -483,7 +483,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Gotowe</t>
+          <t>W trakcie</t>
         </is>
       </c>
     </row>
@@ -499,7 +499,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Gotowe</t>
+          <t>W trakcie</t>
         </is>
       </c>
     </row>
@@ -515,7 +515,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Gotowe</t>
+          <t>W trakcie</t>
         </is>
       </c>
     </row>
@@ -530,6 +530,134 @@
         </is>
       </c>
       <c r="D6" t="inlineStr">
+        <is>
+          <t>W trakcie</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>prd.T2_600_250_20_15.dld</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>W trakcie</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>prd.T3g_4_100_50_50.dld</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Gotowe</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>prd.T40034102p4p5.dld</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>W trakcie</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>prd.T40034912p1i2.dld</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>W trakcie</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>prd.T40062106.dld</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Gotowe</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>prd.T40662901siatka.dld</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Gotowe</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>prd.T4_100k9050.dld</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Gotowe</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>prd.T8_300_100_50_.dld</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>Gotowe</t>
         </is>

</xml_diff>

<commit_message>
POPRAWIONY MANGER, zapis excel
</commit_message>
<xml_diff>
--- a/testy_MANAGER_GIECIA/ListaElementow.xlsx
+++ b/testy_MANAGER_GIECIA/ListaElementow.xlsx
@@ -431,7 +431,13 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="4" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="26" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -462,7 +468,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>prd.40034102p4p5.dld</t>
+          <t>9.dld</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -563,7 +569,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Gotowe</t>
+          <t>W trakcie</t>
         </is>
       </c>
     </row>
@@ -595,7 +601,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>W trakcie</t>
+          <t>Gotowe</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
POPRAWIONY MANGER, FOLDER DELEM
</commit_message>
<xml_diff>
--- a/testy_MANAGER_GIECIA/ListaElementow.xlsx
+++ b/testy_MANAGER_GIECIA/ListaElementow.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,9 +433,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="4" customWidth="1" min="1" max="1"/>
+    <col width="5" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="26" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
@@ -463,12 +463,12 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>9.dld</t>
+          <t>man.manualmode.dld</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -479,28 +479,28 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>prd.40034912p1i2.dld</t>
+          <t>prd.2_600_250_20_15.dld</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>W trakcie</t>
+          <t>Archiwum</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>prd.8_300_100_50_.dld</t>
+          <t>prd.3g_4_100_50_50.dld</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -511,23 +511,23 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>prd.40062106.dld</t>
+          <t>prd.40034102p4p5.dld</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>W trakcie</t>
+          <t>Archiwum</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
@@ -537,133 +537,101 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>W trakcie</t>
+          <t>Archiwum</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>prd.T2_600_250_20_15.dld</t>
+          <t>prd.4_100k9050.dld</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>W trakcie</t>
+          <t>Archiwum</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>prd.T3g_4_100_50_50.dld</t>
+          <t>prd.8_300_100_50_.dld</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>W trakcie</t>
+          <t>Archiwum</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>prd.T40034102p4p5.dld</t>
+          <t>prd.GRAFIKA.dld</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>W trakcie</t>
+          <t>Archiwum</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>prd.T40034912p1i2.dld</t>
+          <t>prd.testTrakcie.dld</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Gotowe</t>
+          <t>Archiwum</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>prd.T40062106.dld</t>
+          <t>prd.TEST1.dld</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Gotowe</t>
+          <t>W trakcie</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>prd.T40662901siatka.dld</t>
+          <t>prd.626246TESAT.dld</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
-        <is>
-          <t>Gotowe</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>prd.T4_100k9050.dld</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Gotowe</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>prd.T8_300_100_50_.dld</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
         <is>
           <t>Gotowe</t>
         </is>

</xml_diff>